<commit_message>
[GAZ-002] TypScript Interfaces and Panels
</commit_message>
<xml_diff>
--- a/docs/Job Seeker Diagnostic model.xlsx
+++ b/docs/Job Seeker Diagnostic model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19680"/>
   </bookViews>
   <sheets>
     <sheet name="EA QUESTIONNAIRE" sheetId="7" r:id="rId1"/>
@@ -670,7 +670,7 @@
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,6 +719,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -864,10 +880,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1073,8 +1123,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="37">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1552,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1575,8 +1659,14 @@
     <col min="20" max="20" width="60.75" style="33" customWidth="1"/>
     <col min="21" max="21" width="36.75" style="10" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="49.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="32" width="8.625" style="10"/>
+    <col min="23" max="23" width="27.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="8.625" style="10"/>
     <col min="33" max="33" width="8.625" style="10" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.625" style="10"/>
     <col min="35" max="35" width="20" style="10" bestFit="1" customWidth="1"/>
@@ -3047,7 +3137,7 @@
     <mergeCell ref="R39:R51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -3077,8 +3167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>